<commit_message>
Updating marking sheet and removing comment
</commit_message>
<xml_diff>
--- a/docs/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/docs/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Google Drive/BIT/Term 5/Full Stack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Google Drive/BIT/Term 5/Full Stack/full_stack_assignments/game_pit/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E2E409-7C97-BC48-A313-89E28837FD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FB4E6E-7BCF-B548-8F65-E86B88491BCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46840" yWindow="12640" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="219">
   <si>
     <t>Confirm</t>
   </si>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t xml:space="preserve">Active Storage uploads are stored to Google Cloud or AWS S3. </t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1479,8 @@
   <dimension ref="A1:AC1122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1494,7 +1497,7 @@
     <row r="1" spans="1:29" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I173 &amp; "  /  Verified: " &amp; J173 &amp; "  /  Verified with Deductions: " &amp; K173 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L173</f>
-        <v>Unverified Marks: 102  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
+        <v>Unverified Marks: 114  /  Verified: 56  /  Verified with Deductions: 47  /  Verified with Deductions &amp; Milestones: 47</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1618,7 +1621,7 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G4" s="26">
         <v>2</v>
@@ -1632,11 +1635,11 @@
       </c>
       <c r="J4" s="21">
         <f t="shared" ref="J4:J5" si="1">IF(F4 = "yes",G4, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="21">
         <f t="shared" ref="K4:K5" si="2">IF(F4 = "yes",G4, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
@@ -1668,7 +1671,7 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
@@ -1682,11 +1685,11 @@
       </c>
       <c r="J5" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="21">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -1715,7 +1718,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F6" s="29"/>
       <c r="G6" s="30"/>
@@ -1750,7 +1753,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="30"/>
@@ -1788,7 +1791,7 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G8" s="26">
         <v>2</v>
@@ -1800,11 +1803,11 @@
       </c>
       <c r="J8" s="21">
         <f t="shared" ref="J8:J9" si="4">IF(F8 = "yes",G8, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="21">
         <f t="shared" ref="K8:K9" si="5">IF(F8 = "yes",G8, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
@@ -1836,7 +1839,7 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="G9" s="26">
         <v>2</v>
@@ -1844,15 +1847,15 @@
       <c r="H9" s="31"/>
       <c r="I9" s="21">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
@@ -1881,7 +1884,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="30"/>
@@ -1916,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="30"/>
@@ -1954,7 +1957,7 @@
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G12" s="26">
         <v>2</v>
@@ -1966,11 +1969,11 @@
       </c>
       <c r="J12" s="21">
         <f>IF(F12 = "yes",G12, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="21">
         <f>IF(F12 = "yes",G12, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
@@ -2035,7 +2038,7 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G14" s="26">
         <v>2</v>
@@ -2047,11 +2050,11 @@
       </c>
       <c r="J14" s="21">
         <f>IF(F14 = "yes",G14, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="21">
         <f>IF(F14 = "yes",G14, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
@@ -2080,7 +2083,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="30"/>
@@ -2118,7 +2121,7 @@
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G16" s="26">
         <v>4</v>
@@ -2130,11 +2133,11 @@
       </c>
       <c r="J16" s="21">
         <f>IF(F16 = "yes",G16, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K16" s="21">
         <f>IF(F16 = "yes",G16, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -2232,7 +2235,7 @@
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G19" s="26">
         <v>2</v>
@@ -2246,11 +2249,11 @@
       </c>
       <c r="J19" s="21">
         <f t="shared" ref="J19:J20" si="7">IF(F19 = "yes",G19, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19" s="21">
         <f>IF(F19 = "yes",G19, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
@@ -2400,7 +2403,7 @@
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G23" s="26">
         <v>2</v>
@@ -2414,11 +2417,11 @@
       </c>
       <c r="J23" s="21">
         <f t="shared" ref="J23:J24" si="9">IF(F23 = "yes",G23, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23" s="21">
         <f>IF(F23 = "yes",G23, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
@@ -2450,7 +2453,7 @@
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="25" t="s">
-        <v>12</v>
+        <v>216</v>
       </c>
       <c r="G24" s="26">
         <v>2</v>
@@ -2458,7 +2461,7 @@
       <c r="H24" s="31"/>
       <c r="I24" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="21">
         <f t="shared" si="9"/>
@@ -2638,7 +2641,7 @@
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G29" s="26">
         <v>2</v>
@@ -2650,11 +2653,11 @@
       </c>
       <c r="J29" s="21">
         <f t="shared" ref="J29:J30" si="11">IF(F29 = "yes",G29, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K29" s="21">
         <f>IF(F29 = "yes",G29, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L29" s="22"/>
       <c r="M29" s="22"/>
@@ -3012,7 +3015,7 @@
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G39" s="26">
         <v>4</v>
@@ -3026,11 +3029,11 @@
       </c>
       <c r="J39" s="21">
         <f t="shared" ref="J39:J40" si="13">IF(F39 = "yes",G39, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K39" s="21">
         <f>IF(F39 = "yes",G39, $M$2)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
@@ -3062,7 +3065,7 @@
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G40" s="26">
         <v>4</v>
@@ -3074,11 +3077,11 @@
       </c>
       <c r="J40" s="21">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40" s="21">
         <f>IF(F40 = "yes",G40, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
@@ -3106,7 +3109,7 @@
         <v>63</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F41" s="29"/>
       <c r="G41" s="33"/>
@@ -3141,7 +3144,7 @@
         <v>64</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="33"/>
@@ -3176,7 +3179,7 @@
         <v>65</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F43" s="29"/>
       <c r="G43" s="33"/>
@@ -4152,7 +4155,7 @@
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="G69" s="26">
         <v>2</v>
@@ -4160,15 +4163,15 @@
       <c r="H69" s="31"/>
       <c r="I69" s="21">
         <f>IF(OR(F69 = "maybe", F69 = "yes"),G69, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" s="21">
         <f>IF(F69 = "yes",G69, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K69" s="21">
         <f>IF(F69 = "yes",G69, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
@@ -4491,7 +4494,7 @@
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G78" s="26">
         <v>2</v>
@@ -4503,11 +4506,11 @@
       </c>
       <c r="J78" s="21">
         <f>IF(F78 = "yes",G78, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K78" s="21">
         <f>IF(F78 = "yes",G78, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L78" s="22"/>
       <c r="M78" s="22"/>
@@ -4536,7 +4539,7 @@
         <v>108</v>
       </c>
       <c r="E79" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F79" s="29"/>
       <c r="G79" s="33"/>
@@ -5065,7 +5068,7 @@
       </c>
       <c r="E93" s="11"/>
       <c r="F93" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G93" s="26">
         <v>2</v>
@@ -5079,11 +5082,11 @@
       </c>
       <c r="J93" s="21">
         <f t="shared" ref="J93:J94" si="15">IF(F93 = "yes",G93, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K93" s="21">
         <f>IF(F93 = "yes",G93, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L93" s="22"/>
       <c r="M93" s="22"/>
@@ -5812,7 +5815,7 @@
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="57" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G112" s="26">
         <v>2</v>
@@ -5824,11 +5827,11 @@
       </c>
       <c r="J112" s="21">
         <f t="shared" ref="J112:J115" si="17">IF(F112 = "yes",G112, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K112" s="21">
         <f t="shared" ref="K112:K115" si="18">IF(F112 = "yes",G112, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L112" s="22"/>
       <c r="M112" s="22"/>
@@ -5908,7 +5911,7 @@
       </c>
       <c r="E114" s="11"/>
       <c r="F114" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="G114" s="26">
         <v>2</v>
@@ -5916,15 +5919,15 @@
       <c r="H114" s="31"/>
       <c r="I114" s="21">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J114" s="21">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K114" s="21">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L114" s="22"/>
       <c r="M114" s="22"/>
@@ -6123,7 +6126,7 @@
       </c>
       <c r="E119" s="11"/>
       <c r="F119" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G119" s="26">
         <v>8</v>
@@ -6135,11 +6138,11 @@
       </c>
       <c r="J119" s="21">
         <f>IF(F119 = "yes",G119, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K119" s="21">
         <f>IF(F119 = "yes",G119, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L119" s="22"/>
       <c r="M119" s="22"/>
@@ -6272,7 +6275,7 @@
       </c>
       <c r="E123" s="11"/>
       <c r="F123" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G123" s="26">
         <v>4</v>
@@ -6286,11 +6289,11 @@
       </c>
       <c r="J123" s="21">
         <f>IF(F123 = "yes",G123, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K123" s="21">
         <f>IF(F123 = "yes",G123, $M$2)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L123" s="22"/>
       <c r="M123" s="22"/>
@@ -6319,7 +6322,7 @@
         <v>163</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F124" s="29"/>
       <c r="G124" s="33"/>
@@ -6354,7 +6357,7 @@
         <v>164</v>
       </c>
       <c r="E125" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F125" s="29"/>
       <c r="G125" s="33"/>
@@ -6389,7 +6392,7 @@
         <v>165</v>
       </c>
       <c r="E126" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F126" s="29"/>
       <c r="G126" s="33"/>
@@ -6424,7 +6427,7 @@
         <v>166</v>
       </c>
       <c r="E127" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F127" s="29"/>
       <c r="G127" s="33"/>
@@ -6459,7 +6462,7 @@
         <v>167</v>
       </c>
       <c r="E128" s="25" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="F128" s="29"/>
       <c r="G128" s="33"/>
@@ -6497,7 +6500,7 @@
       </c>
       <c r="E129" s="11"/>
       <c r="F129" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G129" s="26">
         <v>4</v>
@@ -6509,11 +6512,11 @@
       </c>
       <c r="J129" s="21">
         <f t="shared" ref="J129:J131" si="20">IF(F129 = "yes",G129, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K129" s="21">
         <f t="shared" ref="K129:K131" si="21">IF(F129 = "yes",G129, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L129" s="22"/>
       <c r="M129" s="22"/>
@@ -7226,7 +7229,7 @@
       </c>
       <c r="E148" s="11"/>
       <c r="F148" s="25" t="s">
-        <v>12</v>
+        <v>216</v>
       </c>
       <c r="G148" s="26">
         <v>4</v>
@@ -7234,7 +7237,7 @@
       <c r="H148" s="31"/>
       <c r="I148" s="21">
         <f>IF(OR(F148 = "maybe", F148 = "yes"),G148, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J148" s="21">
         <f>IF(F148 = "yes",G148, 0)</f>
@@ -8142,19 +8145,19 @@
       <c r="H173" s="11"/>
       <c r="I173" s="56">
         <f t="shared" ref="I173:K173" si="23">SUM(I4:I165)</f>
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="J173" s="21">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K173" s="21">
         <f t="shared" si="23"/>
-        <v>-30</v>
+        <v>47</v>
       </c>
       <c r="L173" s="21">
         <f>CHOOSE(SUM(L168:L171)+1, MIN(60, K173) + (K173 - MIN(60, K173))/2,MIN(70, KJ173) + (K173 - MIN(70, K173))/2,MIN(80, K173) + (K173 - MIN(80, K173))/2,MIN(90, K173) + (K173 - MIN(90, K173))/2, K173)</f>
-        <v>-30</v>
+        <v>47</v>
       </c>
       <c r="M173" s="22"/>
       <c r="N173" s="8"/>

</xml_diff>